<commit_message>
commit -m "as on 20Oct2019"
</commit_message>
<xml_diff>
--- a/Additonal_Utility/Down_Scripts_List.xlsx
+++ b/Additonal_Utility/Down_Scripts_List.xlsx
@@ -346,10 +346,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1375"/>
+  <dimension ref="A1:C1658"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C1375"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
@@ -701,7 +701,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -971,7 +971,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -2591,7 +2591,7 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -2831,7 +2831,7 @@
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -3431,7 +3431,7 @@
       </c>
       <c r="C205" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -3521,7 +3521,7 @@
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -3536,7 +3536,7 @@
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -3776,7 +3776,7 @@
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -4001,7 +4001,7 @@
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -4046,7 +4046,7 @@
       </c>
       <c r="C246" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -4781,7 +4781,7 @@
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -6746,7 +6746,7 @@
       </c>
       <c r="C426" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -7301,7 +7301,7 @@
       </c>
       <c r="C463" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -10856,7 +10856,7 @@
       </c>
       <c r="C700" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -11351,7 +11351,7 @@
       </c>
       <c r="C733" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -12326,7 +12326,7 @@
       </c>
       <c r="C798" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -13301,7 +13301,7 @@
       </c>
       <c r="C863" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -13781,7 +13781,7 @@
       </c>
       <c r="C895" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -14501,7 +14501,7 @@
       </c>
       <c r="C943" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -14741,7 +14741,7 @@
       </c>
       <c r="C959" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -14996,7 +14996,7 @@
       </c>
       <c r="C976" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -15011,7 +15011,7 @@
       </c>
       <c r="C977" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -16226,7 +16226,7 @@
       </c>
       <c r="C1058" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -17651,7 +17651,7 @@
       </c>
       <c r="C1153" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -18116,7 +18116,7 @@
       </c>
       <c r="C1184" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -18731,7 +18731,7 @@
       </c>
       <c r="C1225" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
     </row>
@@ -20711,7 +20711,7 @@
       </c>
       <c r="C1357" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
     </row>
@@ -20980,6 +20980,3402 @@
         <v>17519</v>
       </c>
       <c r="C1375" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1376">
+      <c r="A1376" t="inlineStr">
+        <is>
+          <t>APCL</t>
+        </is>
+      </c>
+      <c r="C1376" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1377">
+      <c r="A1377" t="inlineStr">
+        <is>
+          <t>ARENTERP</t>
+        </is>
+      </c>
+      <c r="C1377" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1378">
+      <c r="A1378" t="inlineStr">
+        <is>
+          <t>ASAHISONG</t>
+        </is>
+      </c>
+      <c r="C1378" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1379">
+      <c r="A1379" t="inlineStr">
+        <is>
+          <t>ASIANHOTNR</t>
+        </is>
+      </c>
+      <c r="C1379" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1380">
+      <c r="A1380" t="inlineStr">
+        <is>
+          <t>ASPINWALL</t>
+        </is>
+      </c>
+      <c r="C1380" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1381">
+      <c r="A1381" t="inlineStr">
+        <is>
+          <t>ATLASCYCLE</t>
+        </is>
+      </c>
+      <c r="C1381" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1382">
+      <c r="A1382" t="inlineStr">
+        <is>
+          <t>ATNINTER</t>
+        </is>
+      </c>
+      <c r="C1382" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1383">
+      <c r="A1383" t="inlineStr">
+        <is>
+          <t>AXISGOLD</t>
+        </is>
+      </c>
+      <c r="C1383" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1384">
+      <c r="A1384" t="inlineStr">
+        <is>
+          <t>AXISNIFTY</t>
+        </is>
+      </c>
+      <c r="C1384" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1385">
+      <c r="A1385" t="inlineStr">
+        <is>
+          <t>BALAXI</t>
+        </is>
+      </c>
+      <c r="C1385" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1386">
+      <c r="A1386" t="inlineStr">
+        <is>
+          <t>BANARISUG</t>
+        </is>
+      </c>
+      <c r="C1386" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1387">
+      <c r="A1387" t="inlineStr">
+        <is>
+          <t>BASML</t>
+        </is>
+      </c>
+      <c r="C1387" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1388">
+      <c r="A1388" t="inlineStr">
+        <is>
+          <t>BAYERCROP</t>
+        </is>
+      </c>
+      <c r="C1388" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1389">
+      <c r="A1389" t="inlineStr">
+        <is>
+          <t>BEARDSELL</t>
+        </is>
+      </c>
+      <c r="C1389" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1390">
+      <c r="A1390" t="inlineStr">
+        <is>
+          <t>BHARATRAS</t>
+        </is>
+      </c>
+      <c r="C1390" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1391">
+      <c r="A1391" t="inlineStr">
+        <is>
+          <t>BIL</t>
+        </is>
+      </c>
+      <c r="C1391" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1392">
+      <c r="A1392" t="inlineStr">
+        <is>
+          <t>BIOFILCHEM</t>
+        </is>
+      </c>
+      <c r="C1392" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1393">
+      <c r="A1393" t="inlineStr">
+        <is>
+          <t>BLUEBLENDS</t>
+        </is>
+      </c>
+      <c r="C1393" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1394">
+      <c r="A1394" t="inlineStr">
+        <is>
+          <t>BLUECHIP</t>
+        </is>
+      </c>
+      <c r="C1394" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1395">
+      <c r="A1395" t="inlineStr">
+        <is>
+          <t>BLUECOAST</t>
+        </is>
+      </c>
+      <c r="C1395" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1396">
+      <c r="A1396" t="inlineStr">
+        <is>
+          <t>BLUEDART</t>
+        </is>
+      </c>
+      <c r="C1396" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1397">
+      <c r="A1397" t="inlineStr">
+        <is>
+          <t>BSLGOLDETF</t>
+        </is>
+      </c>
+      <c r="C1397" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1398">
+      <c r="A1398" t="inlineStr">
+        <is>
+          <t>BSLNIFTY</t>
+        </is>
+      </c>
+      <c r="C1398" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1399">
+      <c r="A1399" t="inlineStr">
+        <is>
+          <t>BVCL</t>
+        </is>
+      </c>
+      <c r="C1399" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1400">
+      <c r="A1400" t="inlineStr">
+        <is>
+          <t>CAPTRUST</t>
+        </is>
+      </c>
+      <c r="C1400" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1401">
+      <c r="A1401" t="inlineStr">
+        <is>
+          <t>CENTUM</t>
+        </is>
+      </c>
+      <c r="C1401" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1402">
+      <c r="A1402" t="inlineStr">
+        <is>
+          <t>CERA</t>
+        </is>
+      </c>
+      <c r="C1402" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1403">
+      <c r="A1403" t="inlineStr">
+        <is>
+          <t>CHEMFAB</t>
+        </is>
+      </c>
+      <c r="C1403" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1404">
+      <c r="A1404" t="inlineStr">
+        <is>
+          <t>CINEVISTA</t>
+        </is>
+      </c>
+      <c r="C1404" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1405">
+      <c r="A1405" t="inlineStr">
+        <is>
+          <t>CLEDUCATE</t>
+        </is>
+      </c>
+      <c r="C1405" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1406">
+      <c r="A1406" t="inlineStr">
+        <is>
+          <t>CONSOFINVT</t>
+        </is>
+      </c>
+      <c r="C1406" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1407">
+      <c r="A1407" t="inlineStr">
+        <is>
+          <t>CPSEETF</t>
+        </is>
+      </c>
+      <c r="C1407" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1408">
+      <c r="A1408" t="inlineStr">
+        <is>
+          <t>CREATIVEYE</t>
+        </is>
+      </c>
+      <c r="C1408" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1409">
+      <c r="A1409" t="inlineStr">
+        <is>
+          <t>CRMFGETF</t>
+        </is>
+      </c>
+      <c r="C1409" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1410">
+      <c r="A1410" t="inlineStr">
+        <is>
+          <t>CTE</t>
+        </is>
+      </c>
+      <c r="C1410" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1411">
+      <c r="A1411" t="inlineStr">
+        <is>
+          <t>CUBEXTUB</t>
+        </is>
+      </c>
+      <c r="C1411" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1412">
+      <c r="A1412" t="inlineStr">
+        <is>
+          <t>CURATECH</t>
+        </is>
+      </c>
+      <c r="C1412" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1413">
+      <c r="A1413" t="inlineStr">
+        <is>
+          <t>CYBERMEDIA</t>
+        </is>
+      </c>
+      <c r="C1413" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1414">
+      <c r="A1414" t="inlineStr">
+        <is>
+          <t>DBSTOCKBRO</t>
+        </is>
+      </c>
+      <c r="C1414" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1415">
+      <c r="A1415" t="inlineStr">
+        <is>
+          <t>DCMFINSERV</t>
+        </is>
+      </c>
+      <c r="C1415" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1416">
+      <c r="A1416" t="inlineStr">
+        <is>
+          <t>DCMNVL</t>
+        </is>
+      </c>
+      <c r="C1416" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1417">
+      <c r="A1417" t="inlineStr">
+        <is>
+          <t>DECCANCE</t>
+        </is>
+      </c>
+      <c r="C1417" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1418">
+      <c r="A1418" t="inlineStr">
+        <is>
+          <t>DELTAMAGNT</t>
+        </is>
+      </c>
+      <c r="C1418" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1419">
+      <c r="A1419" t="inlineStr">
+        <is>
+          <t>DFMFOODS</t>
+        </is>
+      </c>
+      <c r="C1419" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1420">
+      <c r="A1420" t="inlineStr">
+        <is>
+          <t>DHUNINV</t>
+        </is>
+      </c>
+      <c r="C1420" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1421">
+      <c r="A1421" t="inlineStr">
+        <is>
+          <t>DICIND</t>
+        </is>
+      </c>
+      <c r="C1421" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1422">
+      <c r="A1422" t="inlineStr">
+        <is>
+          <t>DYNAMATECH</t>
+        </is>
+      </c>
+      <c r="C1422" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1423">
+      <c r="A1423" t="inlineStr">
+        <is>
+          <t>EBANK</t>
+        </is>
+      </c>
+      <c r="C1423" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1424">
+      <c r="A1424" t="inlineStr">
+        <is>
+          <t>EIMCOELECO</t>
+        </is>
+      </c>
+      <c r="C1424" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1425">
+      <c r="A1425" t="inlineStr">
+        <is>
+          <t>EMAMIPAP</t>
+        </is>
+      </c>
+      <c r="C1425" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1426">
+      <c r="A1426" t="inlineStr">
+        <is>
+          <t>EQ30</t>
+        </is>
+      </c>
+      <c r="C1426" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1427">
+      <c r="A1427" t="inlineStr">
+        <is>
+          <t>ESABINDIA</t>
+        </is>
+      </c>
+      <c r="C1427" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1428">
+      <c r="A1428" t="inlineStr">
+        <is>
+          <t>EUROMULTI</t>
+        </is>
+      </c>
+      <c r="C1428" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1429">
+      <c r="A1429" t="inlineStr">
+        <is>
+          <t>EUROTEXIND</t>
+        </is>
+      </c>
+      <c r="C1429" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1430">
+      <c r="A1430" t="inlineStr">
+        <is>
+          <t>EXCELCROP</t>
+        </is>
+      </c>
+      <c r="C1430" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1431">
+      <c r="A1431" t="inlineStr">
+        <is>
+          <t>EXPLEOSOL</t>
+        </is>
+      </c>
+      <c r="C1431" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1432">
+      <c r="A1432" t="inlineStr">
+        <is>
+          <t>FOSECOIND</t>
+        </is>
+      </c>
+      <c r="C1432" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1433">
+      <c r="A1433" t="inlineStr">
+        <is>
+          <t>GANDHITUBE</t>
+        </is>
+      </c>
+      <c r="C1433" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1434">
+      <c r="A1434" t="inlineStr">
+        <is>
+          <t>GANGESSECU</t>
+        </is>
+      </c>
+      <c r="C1434" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1435">
+      <c r="A1435" t="inlineStr">
+        <is>
+          <t>GFSTEELS</t>
+        </is>
+      </c>
+      <c r="C1435" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1436">
+      <c r="A1436" t="inlineStr">
+        <is>
+          <t>GILLANDERS</t>
+        </is>
+      </c>
+      <c r="C1436" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1437">
+      <c r="A1437" t="inlineStr">
+        <is>
+          <t>GILLETTE</t>
+        </is>
+      </c>
+      <c r="C1437" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1438">
+      <c r="A1438" t="inlineStr">
+        <is>
+          <t>GISOLUTION</t>
+        </is>
+      </c>
+      <c r="C1438" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1439">
+      <c r="A1439" t="inlineStr">
+        <is>
+          <t>GKWLIMITED</t>
+        </is>
+      </c>
+      <c r="C1439" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1440">
+      <c r="A1440" t="inlineStr">
+        <is>
+          <t>GLFL</t>
+        </is>
+      </c>
+      <c r="C1440" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1441">
+      <c r="A1441" t="inlineStr">
+        <is>
+          <t>GMMPFAUDLR</t>
+        </is>
+      </c>
+      <c r="C1441" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1442">
+      <c r="A1442" t="inlineStr">
+        <is>
+          <t>GOCLCORP</t>
+        </is>
+      </c>
+      <c r="C1442" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1443">
+      <c r="A1443" t="inlineStr">
+        <is>
+          <t>GOLDENTOBC</t>
+        </is>
+      </c>
+      <c r="C1443" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1444">
+      <c r="A1444" t="inlineStr">
+        <is>
+          <t>GOLDSHARE</t>
+        </is>
+      </c>
+      <c r="C1444" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1445">
+      <c r="A1445" t="inlineStr">
+        <is>
+          <t>GREENLAM</t>
+        </is>
+      </c>
+      <c r="C1445" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1446">
+      <c r="A1446" t="inlineStr">
+        <is>
+          <t>GROBTEA</t>
+        </is>
+      </c>
+      <c r="C1446" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1447">
+      <c r="A1447" t="inlineStr">
+        <is>
+          <t>GRPLTD</t>
+        </is>
+      </c>
+      <c r="C1447" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1448">
+      <c r="A1448" t="inlineStr">
+        <is>
+          <t>GTNTEX</t>
+        </is>
+      </c>
+      <c r="C1448" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1449">
+      <c r="A1449" t="inlineStr">
+        <is>
+          <t>GUJAPOLLO</t>
+        </is>
+      </c>
+      <c r="C1449" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1450">
+      <c r="A1450" t="inlineStr">
+        <is>
+          <t>GUJRAFFIA</t>
+        </is>
+      </c>
+      <c r="C1450" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1451">
+      <c r="A1451" t="inlineStr">
+        <is>
+          <t>HARITASEAT</t>
+        </is>
+      </c>
+      <c r="C1451" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1452">
+      <c r="A1452" t="inlineStr">
+        <is>
+          <t>HAVISHA</t>
+        </is>
+      </c>
+      <c r="C1452" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1453">
+      <c r="A1453" t="inlineStr">
+        <is>
+          <t>HBSL</t>
+        </is>
+      </c>
+      <c r="C1453" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1454">
+      <c r="A1454" t="inlineStr">
+        <is>
+          <t>HDFCMFGETF</t>
+        </is>
+      </c>
+      <c r="C1454" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1455">
+      <c r="A1455" t="inlineStr">
+        <is>
+          <t>HDFCNIFETF</t>
+        </is>
+      </c>
+      <c r="C1455" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1456">
+      <c r="A1456" t="inlineStr">
+        <is>
+          <t>HDFCSENETF</t>
+        </is>
+      </c>
+      <c r="C1456" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1457">
+      <c r="A1457" t="inlineStr">
+        <is>
+          <t>HESTERBIO</t>
+        </is>
+      </c>
+      <c r="C1457" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1458">
+      <c r="A1458" t="inlineStr">
+        <is>
+          <t>HINDCOMPOS</t>
+        </is>
+      </c>
+      <c r="C1458" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1459">
+      <c r="A1459" t="inlineStr">
+        <is>
+          <t>HINDNATGLS</t>
+        </is>
+      </c>
+      <c r="C1459" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1460">
+      <c r="A1460" t="inlineStr">
+        <is>
+          <t>HINDSYNTEX</t>
+        </is>
+      </c>
+      <c r="C1460" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1461">
+      <c r="A1461" t="inlineStr">
+        <is>
+          <t>HISARMETAL</t>
+        </is>
+      </c>
+      <c r="C1461" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1462">
+      <c r="A1462" t="inlineStr">
+        <is>
+          <t>HITECHCORP</t>
+        </is>
+      </c>
+      <c r="C1462" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1463">
+      <c r="A1463" t="inlineStr">
+        <is>
+          <t>HNGSNGBEES</t>
+        </is>
+      </c>
+      <c r="C1463" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1464">
+      <c r="A1464" t="inlineStr">
+        <is>
+          <t>HONAUT</t>
+        </is>
+      </c>
+      <c r="C1464" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1465">
+      <c r="A1465" t="inlineStr">
+        <is>
+          <t>HONDAPOWER</t>
+        </is>
+      </c>
+      <c r="C1465" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1466">
+      <c r="A1466" t="inlineStr">
+        <is>
+          <t>HOTELRUGBY</t>
+        </is>
+      </c>
+      <c r="C1466" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1467">
+      <c r="A1467" t="inlineStr">
+        <is>
+          <t>IBMFNIFTY</t>
+        </is>
+      </c>
+      <c r="C1467" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1468">
+      <c r="A1468" t="inlineStr">
+        <is>
+          <t>ICICI500</t>
+        </is>
+      </c>
+      <c r="C1468" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1469">
+      <c r="A1469" t="inlineStr">
+        <is>
+          <t>ICICIBANKN</t>
+        </is>
+      </c>
+      <c r="C1469" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1470">
+      <c r="A1470" t="inlineStr">
+        <is>
+          <t>ICICILOVOL</t>
+        </is>
+      </c>
+      <c r="C1470" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1471">
+      <c r="A1471" t="inlineStr">
+        <is>
+          <t>ICICINF100</t>
+        </is>
+      </c>
+      <c r="C1471" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1472">
+      <c r="A1472" t="inlineStr">
+        <is>
+          <t>ICICINV20</t>
+        </is>
+      </c>
+      <c r="C1472" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1473">
+      <c r="A1473" t="inlineStr">
+        <is>
+          <t>ICICISENSX</t>
+        </is>
+      </c>
+      <c r="C1473" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1474">
+      <c r="A1474" t="inlineStr">
+        <is>
+          <t>ICRA</t>
+        </is>
+      </c>
+      <c r="C1474" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1475">
+      <c r="A1475" t="inlineStr">
+        <is>
+          <t>IDBIGOLD</t>
+        </is>
+      </c>
+      <c r="C1475" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1476">
+      <c r="A1476" t="inlineStr">
+        <is>
+          <t>IDFNIFTYET</t>
+        </is>
+      </c>
+      <c r="C1476" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1477">
+      <c r="A1477" t="inlineStr">
+        <is>
+          <t>IFBAGRO</t>
+        </is>
+      </c>
+      <c r="C1477" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1478">
+      <c r="A1478" t="inlineStr">
+        <is>
+          <t>IITL</t>
+        </is>
+      </c>
+      <c r="C1478" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1479">
+      <c r="A1479" t="inlineStr">
+        <is>
+          <t>IMPAL</t>
+        </is>
+      </c>
+      <c r="C1479" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1480">
+      <c r="A1480" t="inlineStr">
+        <is>
+          <t>INDIAMART</t>
+        </is>
+      </c>
+      <c r="C1480" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1481">
+      <c r="A1481" t="inlineStr">
+        <is>
+          <t>INDIANCARD</t>
+        </is>
+      </c>
+      <c r="C1481" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1482">
+      <c r="A1482" t="inlineStr">
+        <is>
+          <t>INDLMETER</t>
+        </is>
+      </c>
+      <c r="C1482" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1483">
+      <c r="A1483" t="inlineStr">
+        <is>
+          <t>INDNIPPON</t>
+        </is>
+      </c>
+      <c r="C1483" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1484">
+      <c r="A1484" t="inlineStr">
+        <is>
+          <t>INEOSSTYRO</t>
+        </is>
+      </c>
+      <c r="C1484" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1485">
+      <c r="A1485" t="inlineStr">
+        <is>
+          <t>INFOBEAN</t>
+        </is>
+      </c>
+      <c r="C1485" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1486">
+      <c r="A1486" t="inlineStr">
+        <is>
+          <t>INFRABEES</t>
+        </is>
+      </c>
+      <c r="C1486" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1487">
+      <c r="A1487" t="inlineStr">
+        <is>
+          <t>INTEGRA</t>
+        </is>
+      </c>
+      <c r="C1487" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1488">
+      <c r="A1488" t="inlineStr">
+        <is>
+          <t>IPRU5008</t>
+        </is>
+      </c>
+      <c r="C1488" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="1489">
+      <c r="A1489" t="inlineStr">
+        <is>
+          <t>IVP</t>
+        </is>
+      </c>
+      <c r="C1489" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1490">
+      <c r="A1490" t="inlineStr">
+        <is>
+          <t>IVZINGOLD</t>
+        </is>
+      </c>
+      <c r="C1490" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1491">
+      <c r="A1491" t="inlineStr">
+        <is>
+          <t>IVZINNIFTY</t>
+        </is>
+      </c>
+      <c r="C1491" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1492">
+      <c r="A1492" t="inlineStr">
+        <is>
+          <t>JAIHINDPRO</t>
+        </is>
+      </c>
+      <c r="C1492" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1493">
+      <c r="A1493" t="inlineStr">
+        <is>
+          <t>JCHAC</t>
+        </is>
+      </c>
+      <c r="C1493" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1494">
+      <c r="A1494" t="inlineStr">
+        <is>
+          <t>JIKIND</t>
+        </is>
+      </c>
+      <c r="C1494" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1495">
+      <c r="A1495" t="inlineStr">
+        <is>
+          <t>JINDALPHOT</t>
+        </is>
+      </c>
+      <c r="C1495" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1496">
+      <c r="A1496" t="inlineStr">
+        <is>
+          <t>JMA</t>
+        </is>
+      </c>
+      <c r="C1496" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1497">
+      <c r="A1497" t="inlineStr">
+        <is>
+          <t>JOCIL</t>
+        </is>
+      </c>
+      <c r="C1497" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1498">
+      <c r="A1498" t="inlineStr">
+        <is>
+          <t>JPOLYINVST</t>
+        </is>
+      </c>
+      <c r="C1498" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1499">
+      <c r="A1499" t="inlineStr">
+        <is>
+          <t>JSWHL</t>
+        </is>
+      </c>
+      <c r="C1499" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1500">
+      <c r="A1500" t="inlineStr">
+        <is>
+          <t>KALYANIFRG</t>
+        </is>
+      </c>
+      <c r="C1500" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1501">
+      <c r="A1501" t="inlineStr">
+        <is>
+          <t>KARMAENG</t>
+        </is>
+      </c>
+      <c r="C1501" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1502">
+      <c r="A1502" t="inlineStr">
+        <is>
+          <t>KDDL</t>
+        </is>
+      </c>
+      <c r="C1502" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1503">
+      <c r="A1503" t="inlineStr">
+        <is>
+          <t>KERNEX</t>
+        </is>
+      </c>
+      <c r="C1503" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1504">
+      <c r="A1504" t="inlineStr">
+        <is>
+          <t>KEYFINSERV</t>
+        </is>
+      </c>
+      <c r="C1504" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1505">
+      <c r="A1505" t="inlineStr">
+        <is>
+          <t>KHAITANELE</t>
+        </is>
+      </c>
+      <c r="C1505" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1506">
+      <c r="A1506" t="inlineStr">
+        <is>
+          <t>KHAITANLTD</t>
+        </is>
+      </c>
+      <c r="C1506" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1507">
+      <c r="A1507" t="inlineStr">
+        <is>
+          <t>KHANDSE</t>
+        </is>
+      </c>
+      <c r="C1507" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1508">
+      <c r="A1508" t="inlineStr">
+        <is>
+          <t>KICL</t>
+        </is>
+      </c>
+      <c r="C1508" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1509">
+      <c r="A1509" t="inlineStr">
+        <is>
+          <t>KINGFA</t>
+        </is>
+      </c>
+      <c r="C1509" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1510">
+      <c r="A1510" t="inlineStr">
+        <is>
+          <t>KIRLOSIND</t>
+        </is>
+      </c>
+      <c r="C1510" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1511">
+      <c r="A1511" t="inlineStr">
+        <is>
+          <t>KKCL</t>
+        </is>
+      </c>
+      <c r="C1511" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1512">
+      <c r="A1512" t="inlineStr">
+        <is>
+          <t>KOTAKBKETF</t>
+        </is>
+      </c>
+      <c r="C1512" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1513">
+      <c r="A1513" t="inlineStr">
+        <is>
+          <t>KOTAKNV20</t>
+        </is>
+      </c>
+      <c r="C1513" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1514">
+      <c r="A1514" t="inlineStr">
+        <is>
+          <t>KOTAKPSUBK</t>
+        </is>
+      </c>
+      <c r="C1514" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1515">
+      <c r="A1515" t="inlineStr">
+        <is>
+          <t>KREBSBIO</t>
+        </is>
+      </c>
+      <c r="C1515" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1516">
+      <c r="A1516" t="inlineStr">
+        <is>
+          <t>KSB</t>
+        </is>
+      </c>
+      <c r="C1516" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1517">
+      <c r="A1517" t="inlineStr">
+        <is>
+          <t>LAXMIMACH</t>
+        </is>
+      </c>
+      <c r="C1517" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1518">
+      <c r="A1518" t="inlineStr">
+        <is>
+          <t>LFIC</t>
+        </is>
+      </c>
+      <c r="C1518" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1519">
+      <c r="A1519" t="inlineStr">
+        <is>
+          <t>LGBFORGE</t>
+        </is>
+      </c>
+      <c r="C1519" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1520">
+      <c r="A1520" t="inlineStr">
+        <is>
+          <t>LIBAS</t>
+        </is>
+      </c>
+      <c r="C1520" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1521">
+      <c r="A1521" t="inlineStr">
+        <is>
+          <t>LICNETFGSC</t>
+        </is>
+      </c>
+      <c r="C1521" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1522">
+      <c r="A1522" t="inlineStr">
+        <is>
+          <t>LICNETFN50</t>
+        </is>
+      </c>
+      <c r="C1522" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1523">
+      <c r="A1523" t="inlineStr">
+        <is>
+          <t>LICNETFSEN</t>
+        </is>
+      </c>
+      <c r="C1523" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1524">
+      <c r="A1524" t="inlineStr">
+        <is>
+          <t>LICNFNHGP</t>
+        </is>
+      </c>
+      <c r="C1524" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1525">
+      <c r="A1525" t="inlineStr">
+        <is>
+          <t>LIQUIDETF</t>
+        </is>
+      </c>
+      <c r="C1525" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1526">
+      <c r="A1526" t="inlineStr">
+        <is>
+          <t>LUMAXIND</t>
+        </is>
+      </c>
+      <c r="C1526" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1527">
+      <c r="A1527" t="inlineStr">
+        <is>
+          <t>M50</t>
+        </is>
+      </c>
+      <c r="C1527" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1528">
+      <c r="A1528" t="inlineStr">
+        <is>
+          <t>MAHAPEXLTD</t>
+        </is>
+      </c>
+      <c r="C1528" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1529">
+      <c r="A1529" t="inlineStr">
+        <is>
+          <t>MAHSCOOTER</t>
+        </is>
+      </c>
+      <c r="C1529" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1530">
+      <c r="A1530" t="inlineStr">
+        <is>
+          <t>MAN50ETF</t>
+        </is>
+      </c>
+      <c r="C1530" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1531">
+      <c r="A1531" t="inlineStr">
+        <is>
+          <t>MARATHON</t>
+        </is>
+      </c>
+      <c r="C1531" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1532">
+      <c r="A1532" t="inlineStr">
+        <is>
+          <t>MASKINVEST</t>
+        </is>
+      </c>
+      <c r="C1532" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1533">
+      <c r="A1533" t="inlineStr">
+        <is>
+          <t>MELSTAR</t>
+        </is>
+      </c>
+      <c r="C1533" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1534">
+      <c r="A1534" t="inlineStr">
+        <is>
+          <t>MIL</t>
+        </is>
+      </c>
+      <c r="C1534" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="1535">
+      <c r="A1535" t="inlineStr">
+        <is>
+          <t>MODIRUBBER</t>
+        </is>
+      </c>
+      <c r="C1535" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1536">
+      <c r="A1536" t="inlineStr">
+        <is>
+          <t>MONSANTO</t>
+        </is>
+      </c>
+      <c r="C1536" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1537">
+      <c r="A1537" t="inlineStr">
+        <is>
+          <t>MOTOGENFIN</t>
+        </is>
+      </c>
+      <c r="C1537" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1538">
+      <c r="A1538" t="inlineStr">
+        <is>
+          <t>MPSLTD</t>
+        </is>
+      </c>
+      <c r="C1538" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1539">
+      <c r="A1539" t="inlineStr">
+        <is>
+          <t>MRF</t>
+        </is>
+      </c>
+      <c r="C1539" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1540">
+      <c r="A1540" t="inlineStr">
+        <is>
+          <t>MRO-TEK</t>
+        </is>
+      </c>
+      <c r="C1540" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1541">
+      <c r="A1541" t="inlineStr">
+        <is>
+          <t>N100</t>
+        </is>
+      </c>
+      <c r="C1541" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1542">
+      <c r="A1542" t="inlineStr">
+        <is>
+          <t>NBIFIN</t>
+        </is>
+      </c>
+      <c r="C1542" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1543">
+      <c r="A1543" t="inlineStr">
+        <is>
+          <t>NDGL</t>
+        </is>
+      </c>
+      <c r="C1543" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1544">
+      <c r="A1544" t="inlineStr">
+        <is>
+          <t>NETF</t>
+        </is>
+      </c>
+      <c r="C1544" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1545">
+      <c r="A1545" t="inlineStr">
+        <is>
+          <t>NIFTYEES</t>
+        </is>
+      </c>
+      <c r="C1545" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1546">
+      <c r="A1546" t="inlineStr">
+        <is>
+          <t>NIPPOBATRY</t>
+        </is>
+      </c>
+      <c r="C1546" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1547">
+      <c r="A1547" t="inlineStr">
+        <is>
+          <t>NKIND</t>
+        </is>
+      </c>
+      <c r="C1547" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1548">
+      <c r="A1548" t="inlineStr">
+        <is>
+          <t>NORBTEAEXP</t>
+        </is>
+      </c>
+      <c r="C1548" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1549">
+      <c r="A1549" t="inlineStr">
+        <is>
+          <t>NSIL</t>
+        </is>
+      </c>
+      <c r="C1549" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1550">
+      <c r="A1550" t="inlineStr">
+        <is>
+          <t>OAL</t>
+        </is>
+      </c>
+      <c r="C1550" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1551">
+      <c r="A1551" t="inlineStr">
+        <is>
+          <t>OCCL</t>
+        </is>
+      </c>
+      <c r="C1551" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1552">
+      <c r="A1552" t="inlineStr">
+        <is>
+          <t>ONELIFECAP</t>
+        </is>
+      </c>
+      <c r="C1552" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1553">
+      <c r="A1553" t="inlineStr">
+        <is>
+          <t>PAEL</t>
+        </is>
+      </c>
+      <c r="C1553" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1554">
+      <c r="A1554" t="inlineStr">
+        <is>
+          <t>PAISALO</t>
+        </is>
+      </c>
+      <c r="C1554" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1555">
+      <c r="A1555" t="inlineStr">
+        <is>
+          <t>PALASHSECU</t>
+        </is>
+      </c>
+      <c r="C1555" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1556">
+      <c r="A1556" t="inlineStr">
+        <is>
+          <t>PDSMFL</t>
+        </is>
+      </c>
+      <c r="C1556" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1557">
+      <c r="A1557" t="inlineStr">
+        <is>
+          <t>PETRONENGG</t>
+        </is>
+      </c>
+      <c r="C1557" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1558">
+      <c r="A1558" t="inlineStr">
+        <is>
+          <t>PGHH</t>
+        </is>
+      </c>
+      <c r="C1558" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1559">
+      <c r="A1559" t="inlineStr">
+        <is>
+          <t>PILANIINVS</t>
+        </is>
+      </c>
+      <c r="C1559" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1560">
+      <c r="A1560" t="inlineStr">
+        <is>
+          <t>PIRPHYTO</t>
+        </is>
+      </c>
+      <c r="C1560" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1561">
+      <c r="A1561" t="inlineStr">
+        <is>
+          <t>PKTEA</t>
+        </is>
+      </c>
+      <c r="C1561" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1562">
+      <c r="A1562" t="inlineStr">
+        <is>
+          <t>PODDARHOUS</t>
+        </is>
+      </c>
+      <c r="C1562" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1563">
+      <c r="A1563" t="inlineStr">
+        <is>
+          <t>PODDARMENT</t>
+        </is>
+      </c>
+      <c r="C1563" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1564">
+      <c r="A1564" t="inlineStr">
+        <is>
+          <t>PONNIERODE</t>
+        </is>
+      </c>
+      <c r="C1564" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1565">
+      <c r="A1565" t="inlineStr">
+        <is>
+          <t>PRECOT</t>
+        </is>
+      </c>
+      <c r="C1565" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1566">
+      <c r="A1566" t="inlineStr">
+        <is>
+          <t>PREMIERPOL</t>
+        </is>
+      </c>
+      <c r="C1566" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1567">
+      <c r="A1567" t="inlineStr">
+        <is>
+          <t>PSUBNKBEES</t>
+        </is>
+      </c>
+      <c r="C1567" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1568">
+      <c r="A1568" t="inlineStr">
+        <is>
+          <t>QGOLDHALF</t>
+        </is>
+      </c>
+      <c r="C1568" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1569">
+      <c r="A1569" t="inlineStr">
+        <is>
+          <t>QNIFTY</t>
+        </is>
+      </c>
+      <c r="C1569" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1570">
+      <c r="A1570" t="inlineStr">
+        <is>
+          <t>QUINTEGRA</t>
+        </is>
+      </c>
+      <c r="C1570" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1571">
+      <c r="A1571" t="inlineStr">
+        <is>
+          <t>RAINBOWPAP</t>
+        </is>
+      </c>
+      <c r="C1571" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1572">
+      <c r="A1572" t="inlineStr">
+        <is>
+          <t>RAJVIR</t>
+        </is>
+      </c>
+      <c r="C1572" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1573">
+      <c r="A1573" t="inlineStr">
+        <is>
+          <t>RAMGOPOLY</t>
+        </is>
+      </c>
+      <c r="C1573" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+    </row>
+    <row r="1574">
+      <c r="A1574" t="inlineStr">
+        <is>
+          <t>RANEENGINE</t>
+        </is>
+      </c>
+      <c r="C1574" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1575">
+      <c r="A1575" t="inlineStr">
+        <is>
+          <t>RANEHOLDIN</t>
+        </is>
+      </c>
+      <c r="C1575" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1576">
+      <c r="A1576" t="inlineStr">
+        <is>
+          <t>REGENCERAM</t>
+        </is>
+      </c>
+      <c r="C1576" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1577">
+      <c r="A1577" t="inlineStr">
+        <is>
+          <t>RELCNX100</t>
+        </is>
+      </c>
+      <c r="C1577" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1578">
+      <c r="A1578" t="inlineStr">
+        <is>
+          <t>RELCONS</t>
+        </is>
+      </c>
+      <c r="C1578" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1579">
+      <c r="A1579" t="inlineStr">
+        <is>
+          <t>RELDIVOPP</t>
+        </is>
+      </c>
+      <c r="C1579" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1580">
+      <c r="A1580" t="inlineStr">
+        <is>
+          <t>RELNV20</t>
+        </is>
+      </c>
+      <c r="C1580" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1581">
+      <c r="A1581" t="inlineStr">
+        <is>
+          <t>REPRO</t>
+        </is>
+      </c>
+      <c r="C1581" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1582">
+      <c r="A1582" t="inlineStr">
+        <is>
+          <t>RETFMID150</t>
+        </is>
+      </c>
+      <c r="C1582" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1583">
+      <c r="A1583" t="inlineStr">
+        <is>
+          <t>REVATHI</t>
+        </is>
+      </c>
+      <c r="C1583" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1584">
+      <c r="A1584" t="inlineStr">
+        <is>
+          <t>RGL</t>
+        </is>
+      </c>
+      <c r="C1584" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1585">
+      <c r="A1585" t="inlineStr">
+        <is>
+          <t>ROHITFERRO</t>
+        </is>
+      </c>
+      <c r="C1585" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1586">
+      <c r="A1586" t="inlineStr">
+        <is>
+          <t>RRSLGETF</t>
+        </is>
+      </c>
+      <c r="C1586" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1587">
+      <c r="A1587" t="inlineStr">
+        <is>
+          <t>SABEVENTS</t>
+        </is>
+      </c>
+      <c r="C1587" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1588">
+      <c r="A1588" t="inlineStr">
+        <is>
+          <t>SAGCEM</t>
+        </is>
+      </c>
+      <c r="C1588" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1589">
+      <c r="A1589" t="inlineStr">
+        <is>
+          <t>SALONA</t>
+        </is>
+      </c>
+      <c r="C1589" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1590">
+      <c r="A1590" t="inlineStr">
+        <is>
+          <t>SANDESH</t>
+        </is>
+      </c>
+      <c r="C1590" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1591">
+      <c r="A1591" t="inlineStr">
+        <is>
+          <t>SANGINITA</t>
+        </is>
+      </c>
+      <c r="C1591" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1592">
+      <c r="A1592" t="inlineStr">
+        <is>
+          <t>SASTASUNDR</t>
+        </is>
+      </c>
+      <c r="C1592" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1593">
+      <c r="A1593" t="inlineStr">
+        <is>
+          <t>SATIA</t>
+        </is>
+      </c>
+      <c r="C1593" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1594">
+      <c r="A1594" t="inlineStr">
+        <is>
+          <t>SBIETFQLTY</t>
+        </is>
+      </c>
+      <c r="C1594" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1595">
+      <c r="A1595" t="inlineStr">
+        <is>
+          <t>SCHAEFFLER</t>
+        </is>
+      </c>
+      <c r="C1595" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1596">
+      <c r="A1596" t="inlineStr">
+        <is>
+          <t>SDBL</t>
+        </is>
+      </c>
+      <c r="C1596" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1597">
+      <c r="A1597" t="inlineStr">
+        <is>
+          <t>SESHAPAPER</t>
+        </is>
+      </c>
+      <c r="C1597" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1598">
+      <c r="A1598" t="inlineStr">
+        <is>
+          <t>SETF10GILT</t>
+        </is>
+      </c>
+      <c r="C1598" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1599">
+      <c r="A1599" t="inlineStr">
+        <is>
+          <t>SETFGOLD</t>
+        </is>
+      </c>
+      <c r="C1599" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1600">
+      <c r="A1600" t="inlineStr">
+        <is>
+          <t>SETFNIF50</t>
+        </is>
+      </c>
+      <c r="C1600" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1601">
+      <c r="A1601" t="inlineStr">
+        <is>
+          <t>SETFNIFBK</t>
+        </is>
+      </c>
+      <c r="C1601" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1602">
+      <c r="A1602" t="inlineStr">
+        <is>
+          <t>SETFNN50</t>
+        </is>
+      </c>
+      <c r="C1602" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1603">
+      <c r="A1603" t="inlineStr">
+        <is>
+          <t>SEYAIND</t>
+        </is>
+      </c>
+      <c r="C1603" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1604">
+      <c r="A1604" t="inlineStr">
+        <is>
+          <t>SHARDAMOTR</t>
+        </is>
+      </c>
+      <c r="C1604" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1605">
+      <c r="A1605" t="inlineStr">
+        <is>
+          <t>SHARIABEES</t>
+        </is>
+      </c>
+      <c r="C1605" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1606">
+      <c r="A1606" t="inlineStr">
+        <is>
+          <t>SHIVAMILLS</t>
+        </is>
+      </c>
+      <c r="C1606" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1607">
+      <c r="A1607" t="inlineStr">
+        <is>
+          <t>SHIVATEX</t>
+        </is>
+      </c>
+      <c r="C1607" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1608">
+      <c r="A1608" t="inlineStr">
+        <is>
+          <t>SHRIPISTON</t>
+        </is>
+      </c>
+      <c r="C1608" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1609">
+      <c r="A1609" t="inlineStr">
+        <is>
+          <t>SHYAMTEL</t>
+        </is>
+      </c>
+      <c r="C1609" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1610">
+      <c r="A1610" t="inlineStr">
+        <is>
+          <t>SIL</t>
+        </is>
+      </c>
+      <c r="C1610" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1611">
+      <c r="A1611" t="inlineStr">
+        <is>
+          <t>SILINV</t>
+        </is>
+      </c>
+      <c r="C1611" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1612">
+      <c r="A1612" t="inlineStr">
+        <is>
+          <t>SIRCA</t>
+        </is>
+      </c>
+      <c r="C1612" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1613">
+      <c r="A1613" t="inlineStr">
+        <is>
+          <t>SOTL</t>
+        </is>
+      </c>
+      <c r="C1613" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1614">
+      <c r="A1614" t="inlineStr">
+        <is>
+          <t>SOUTHWEST</t>
+        </is>
+      </c>
+      <c r="C1614" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1615">
+      <c r="A1615" t="inlineStr">
+        <is>
+          <t>STEELCITY</t>
+        </is>
+      </c>
+      <c r="C1615" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1616">
+      <c r="A1616" t="inlineStr">
+        <is>
+          <t>STINDIA</t>
+        </is>
+      </c>
+      <c r="C1616" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1617">
+      <c r="A1617" t="inlineStr">
+        <is>
+          <t>SUBCAPCITY</t>
+        </is>
+      </c>
+      <c r="C1617" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1618">
+      <c r="A1618" t="inlineStr">
+        <is>
+          <t>SUMMITSEC</t>
+        </is>
+      </c>
+      <c r="C1618" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1619">
+      <c r="A1619" t="inlineStr">
+        <is>
+          <t>SUNCLAYLTD</t>
+        </is>
+      </c>
+      <c r="C1619" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1620">
+      <c r="A1620" t="inlineStr">
+        <is>
+          <t>SUNDRMBRAK</t>
+        </is>
+      </c>
+      <c r="C1620" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1621">
+      <c r="A1621" t="inlineStr">
+        <is>
+          <t>SWARAJENG</t>
+        </is>
+      </c>
+      <c r="C1621" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1622">
+      <c r="A1622" t="inlineStr">
+        <is>
+          <t>SWELECTES</t>
+        </is>
+      </c>
+      <c r="C1622" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1623">
+      <c r="A1623" t="inlineStr">
+        <is>
+          <t>TAINWALCHM</t>
+        </is>
+      </c>
+      <c r="C1623" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1624">
+      <c r="A1624" t="inlineStr">
+        <is>
+          <t>TANTIACONS</t>
+        </is>
+      </c>
+      <c r="C1624" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1625">
+      <c r="A1625" t="inlineStr">
+        <is>
+          <t>TASTYBITE</t>
+        </is>
+      </c>
+      <c r="C1625" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1626">
+      <c r="A1626" t="inlineStr">
+        <is>
+          <t>TCIDEVELOP</t>
+        </is>
+      </c>
+      <c r="C1626" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1627">
+      <c r="A1627" t="inlineStr">
+        <is>
+          <t>TCPLPACK</t>
+        </is>
+      </c>
+      <c r="C1627" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1628">
+      <c r="A1628" t="inlineStr">
+        <is>
+          <t>TECHIN</t>
+        </is>
+      </c>
+      <c r="C1628" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1629">
+      <c r="A1629" t="inlineStr">
+        <is>
+          <t>THEINVEST</t>
+        </is>
+      </c>
+      <c r="C1629" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1630">
+      <c r="A1630" t="inlineStr">
+        <is>
+          <t>THEMISMED</t>
+        </is>
+      </c>
+      <c r="C1630" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1631">
+      <c r="A1631" t="inlineStr">
+        <is>
+          <t>THOMASCOTT</t>
+        </is>
+      </c>
+      <c r="C1631" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1632">
+      <c r="A1632" t="inlineStr">
+        <is>
+          <t>TIDEWATER</t>
+        </is>
+      </c>
+      <c r="C1632" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1633">
+      <c r="A1633" t="inlineStr">
+        <is>
+          <t>TIMESGTY</t>
+        </is>
+      </c>
+      <c r="C1633" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1634">
+      <c r="A1634" t="inlineStr">
+        <is>
+          <t>TNTELE</t>
+        </is>
+      </c>
+      <c r="C1634" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1635">
+      <c r="A1635" t="inlineStr">
+        <is>
+          <t>TTKHLTCARE</t>
+        </is>
+      </c>
+      <c r="C1635" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1636">
+      <c r="A1636" t="inlineStr">
+        <is>
+          <t>TTKPRESTIG</t>
+        </is>
+      </c>
+      <c r="C1636" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1637">
+      <c r="A1637" t="inlineStr">
+        <is>
+          <t>TVSSRICHAK</t>
+        </is>
+      </c>
+      <c r="C1637" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1638">
+      <c r="A1638" t="inlineStr">
+        <is>
+          <t>UMESLTD</t>
+        </is>
+      </c>
+      <c r="C1638" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1639">
+      <c r="A1639" t="inlineStr">
+        <is>
+          <t>UNITEDTEA</t>
+        </is>
+      </c>
+      <c r="C1639" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1640">
+      <c r="A1640" t="inlineStr">
+        <is>
+          <t>VESUVIUS</t>
+        </is>
+      </c>
+      <c r="C1640" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1641">
+      <c r="A1641" t="inlineStr">
+        <is>
+          <t>VHL</t>
+        </is>
+      </c>
+      <c r="C1641" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1642">
+      <c r="A1642" t="inlineStr">
+        <is>
+          <t>VIMALOIL</t>
+        </is>
+      </c>
+      <c r="C1642" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1643">
+      <c r="A1643" t="inlineStr">
+        <is>
+          <t>VOLTAMP</t>
+        </is>
+      </c>
+      <c r="C1643" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1644">
+      <c r="A1644" t="inlineStr">
+        <is>
+          <t>VSTIND</t>
+        </is>
+      </c>
+      <c r="C1644" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1645">
+      <c r="A1645" t="inlineStr">
+        <is>
+          <t>VSTTILLERS</t>
+        </is>
+      </c>
+      <c r="C1645" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1646">
+      <c r="A1646" t="inlineStr">
+        <is>
+          <t>WABCOINDIA</t>
+        </is>
+      </c>
+      <c r="C1646" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1647">
+      <c r="A1647" t="inlineStr">
+        <is>
+          <t>WANBURY</t>
+        </is>
+      </c>
+      <c r="C1647" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1648">
+      <c r="A1648" t="inlineStr">
+        <is>
+          <t>WEIZMANIND</t>
+        </is>
+      </c>
+      <c r="C1648" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1649">
+      <c r="A1649" t="inlineStr">
+        <is>
+          <t>WELINV</t>
+        </is>
+      </c>
+      <c r="C1649" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1650">
+      <c r="A1650" t="inlineStr">
+        <is>
+          <t>WENDT</t>
+        </is>
+      </c>
+      <c r="C1650" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1651">
+      <c r="A1651" t="inlineStr">
+        <is>
+          <t>WHEELS</t>
+        </is>
+      </c>
+      <c r="C1651" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1652">
+      <c r="A1652" t="inlineStr">
+        <is>
+          <t>WILLAMAGOR</t>
+        </is>
+      </c>
+      <c r="C1652" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1653">
+      <c r="A1653" t="inlineStr">
+        <is>
+          <t>WIPL</t>
+        </is>
+      </c>
+      <c r="C1653" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1654">
+      <c r="A1654" t="inlineStr">
+        <is>
+          <t>WSI</t>
+        </is>
+      </c>
+      <c r="C1654" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1655">
+      <c r="A1655" t="inlineStr">
+        <is>
+          <t>XLENERGY</t>
+        </is>
+      </c>
+      <c r="C1655" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1656">
+      <c r="A1656" t="inlineStr">
+        <is>
+          <t>ZENITHEXPO</t>
+        </is>
+      </c>
+      <c r="C1656" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1657">
+      <c r="A1657" t="inlineStr">
+        <is>
+          <t>ZODIACLOTH</t>
+        </is>
+      </c>
+      <c r="C1657" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="1658">
+      <c r="A1658" t="inlineStr">
+        <is>
+          <t>ZODJRDMKJ</t>
+        </is>
+      </c>
+      <c r="C1658" t="inlineStr">
         <is>
           <t>No</t>
         </is>

</xml_diff>